<commit_message>
End of NIght checkin
Stuff
</commit_message>
<xml_diff>
--- a/MI6_FinalProject_Plan.xlsx
+++ b/MI6_FinalProject_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingm\Documents\GitHub\2021FA_SGD285_FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School Assignments\2021FA.SGD.285.2141 - Software Engineering\Project 3 - Final Project\2021FA_SGD285_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FC6A75-4C75-4977-908C-603B18392A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5F7F07-EC15-4F5A-ACF2-4902BB9EDDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Estimated Implementation</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Programming: Enemy AI</t>
+  </si>
+  <si>
+    <t>Ongoing as needed</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -187,6 +190,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -706,51 +712,71 @@
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="8">
+        <v>44524</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="8">
+        <v>44517</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="8">
+        <v>44517</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="8">
+        <v>44524</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">

</xml_diff>